<commit_message>
Better Bosch sensor calibration
</commit_message>
<xml_diff>
--- a/m50,m40,m60 Pnp/M50 temp sensor calibrations.xlsx
+++ b/m50,m40,m60 Pnp/M50 temp sensor calibrations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kemppain\Documents\GitHub\Speeduino-M5x-PCBs\m50,m40,m60 Pnp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m50,m40,m60 Pnp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD1B44E-E829-48E8-8DAD-EF3A2643AE0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE640B1E-F0A9-4D52-A453-EB26843A8D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26520" windowHeight="8445" xr2:uid="{9F799CD1-2A4A-44B5-AD76-2F73834C19F2}"/>
+    <workbookView xWindow="4545" yWindow="2610" windowWidth="21660" windowHeight="15570" xr2:uid="{9F799CD1-2A4A-44B5-AD76-2F73834C19F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Resistance (Ohms)</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Temperature °C</t>
+  </si>
+  <si>
+    <t>Values from stock ecu:</t>
   </si>
 </sst>
 </file>
@@ -113,6 +116,1009 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Temp curve</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$4:$J$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$4:$K$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>323</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>596</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>834</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1175</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1707</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3792</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5896</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9397</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15462</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26114</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45313</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8C57-4E33-AC98-AC48082CDFA5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="590176704"/>
+        <c:axId val="590176376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="590176704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="590176376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="590176376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="590176704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53772DB8-06B2-4CF6-B621-0AFA003D008C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -412,103 +1418,249 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F106746-37D8-4B33-A5C3-5E76D75A3820}">
-  <dimension ref="B1:C13"/>
+  <dimension ref="B1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
         <v>2490</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="J3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="J4" s="1">
+        <v>140</v>
+      </c>
+      <c r="K4" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
-        <v>15</v>
+        <v>-40</v>
       </c>
       <c r="C5" s="1">
-        <v>3150</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+        <v>45313</v>
+      </c>
+      <c r="J5" s="1">
+        <v>130</v>
+      </c>
+      <c r="K5" s="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1">
-        <v>1380</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+        <v>2500</v>
+      </c>
+      <c r="J6" s="1">
+        <v>120</v>
+      </c>
+      <c r="K6" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C7" s="1">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="J7" s="1">
+        <v>110</v>
+      </c>
+      <c r="K7" s="1">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J8" s="1">
+        <v>100</v>
+      </c>
+      <c r="K8" s="1">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="J9" s="1">
+        <v>90</v>
+      </c>
+      <c r="K9" s="1">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="J10" s="1">
+        <v>80</v>
+      </c>
+      <c r="K10" s="1">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
-        <v>0</v>
+        <v>-40</v>
       </c>
       <c r="C11" s="1">
-        <v>5820</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+        <v>45313</v>
+      </c>
+      <c r="J11" s="1">
+        <v>70</v>
+      </c>
+      <c r="K11" s="1">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1">
-        <v>2183</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+        <v>2500</v>
+      </c>
+      <c r="J12" s="1">
+        <v>60</v>
+      </c>
+      <c r="K12" s="1">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>100</v>
       </c>
       <c r="C13" s="1">
-        <v>185</v>
+        <v>187</v>
+      </c>
+      <c r="J13" s="1">
+        <v>50</v>
+      </c>
+      <c r="K13" s="1">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J14" s="1">
+        <v>40</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J15" s="1">
+        <v>30</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J16" s="1">
+        <v>20</v>
+      </c>
+      <c r="K16" s="1">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="17" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J17" s="1">
+        <v>10</v>
+      </c>
+      <c r="K17" s="1">
+        <v>3792</v>
+      </c>
+    </row>
+    <row r="18" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>5896</v>
+      </c>
+    </row>
+    <row r="19" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J19" s="1">
+        <v>-10</v>
+      </c>
+      <c r="K19" s="1">
+        <v>9397</v>
+      </c>
+    </row>
+    <row r="20" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J20" s="1">
+        <v>-20</v>
+      </c>
+      <c r="K20" s="1">
+        <v>15462</v>
+      </c>
+    </row>
+    <row r="21" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J21" s="1">
+        <v>-30</v>
+      </c>
+      <c r="K21" s="1">
+        <v>26114</v>
+      </c>
+    </row>
+    <row r="22" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="1">
+        <v>-40</v>
+      </c>
+      <c r="K22" s="1">
+        <v>45313</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>